<commit_message>
Subiendo documento de datos
</commit_message>
<xml_diff>
--- a/Data/PrecipitacionRD.xlsx
+++ b/Data/PrecipitacionRD.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oai01\Desktop\Documentos recibidos-2  OAI\DATOS ABIERTOS 2024\TRIMESTRE JULIO - SEPT\LISTO SUBIR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ed20dfd5d8431f6e/Documents/APGPAC/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{76BD28E8-0BF0-4F1A-B2AB-83A2B4C73B9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7350"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Precipitacion mensual estacion " sheetId="1" r:id="rId1"/>
@@ -19,79 +20,28 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="4">
   <si>
     <t>ESTACION</t>
-  </si>
-  <si>
-    <t>PRECIPITACION EN MILIMETRO</t>
-  </si>
-  <si>
-    <t>MES</t>
-  </si>
-  <si>
-    <t>AÑO</t>
   </si>
   <si>
     <t>Santo Domingo</t>
   </si>
   <si>
-    <t>Enero</t>
+    <t>FECHA</t>
   </si>
   <si>
-    <t>Febrero</t>
-  </si>
-  <si>
-    <t>Marzo</t>
-  </si>
-  <si>
-    <t>Abril</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mayo </t>
-  </si>
-  <si>
-    <t>Junio</t>
-  </si>
-  <si>
-    <t>Julio</t>
-  </si>
-  <si>
-    <t>Agosto</t>
-  </si>
-  <si>
-    <t>Septiembre</t>
-  </si>
-  <si>
-    <t>Octubre</t>
-  </si>
-  <si>
-    <t>Noviembre</t>
-  </si>
-  <si>
-    <t>Diciembre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Abril </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Junio </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diciembre </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marzo </t>
+    <t>PRECIPITACION</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -222,6 +172,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -573,10 +531,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -597,7 +553,7 @@
     <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
     <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
     <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Buena" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Bueno" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
@@ -897,1165 +853,886 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D82"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="B83" sqref="B83"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="17.88671875" customWidth="1"/>
+    <col min="2" max="2" width="37.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>240</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C2" s="3">
+        <v>43101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>125.7</v>
       </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C3" s="3">
+        <v>43132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B4">
         <v>84.6</v>
       </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C4" s="3">
+        <v>43160</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B5">
         <v>27.4</v>
       </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C5" s="3">
+        <v>43191</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B6">
         <v>120.6</v>
       </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C6" s="3">
+        <v>43221</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B7">
         <v>61.3</v>
       </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C7" s="3">
+        <v>43252</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B8">
         <v>299.8</v>
       </c>
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C8" s="3">
+        <v>43282</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B9">
         <v>182</v>
       </c>
-      <c r="C9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C9" s="3">
+        <v>43313</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B10">
         <v>319.10000000000002</v>
       </c>
-      <c r="C10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="3">
+        <v>43344</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B11">
         <v>112</v>
       </c>
-      <c r="C11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C11" s="3">
+        <v>43374</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B12">
         <v>105.3</v>
       </c>
-      <c r="C12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C12" s="3">
+        <v>43405</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B13">
         <v>22.6</v>
       </c>
-      <c r="C13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C13" s="3">
+        <v>43435</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B14">
         <v>36.6</v>
       </c>
-      <c r="C14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C14" s="3">
+        <v>43466</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B15">
         <v>13.9</v>
       </c>
-      <c r="C15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C15" s="3">
+        <v>43497</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B16">
         <v>36.700000000000003</v>
       </c>
-      <c r="C16" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C16" s="3">
+        <v>43525</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B17">
         <v>40.9</v>
       </c>
-      <c r="C17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C17" s="3">
+        <v>43556</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B18">
         <v>67</v>
       </c>
-      <c r="C18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C18" s="3">
+        <v>43586</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B19">
         <v>9.6</v>
       </c>
-      <c r="C19" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C19" s="3">
+        <v>43617</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B20">
         <v>125.3</v>
       </c>
-      <c r="C20" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C20" s="3">
+        <v>43647</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B21">
         <v>76.8</v>
       </c>
-      <c r="C21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D21">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C21" s="3">
+        <v>43678</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B22">
         <v>87.9</v>
       </c>
-      <c r="C22" t="s">
-        <v>13</v>
-      </c>
-      <c r="D22">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C22" s="3">
+        <v>43709</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B23">
         <v>63.2</v>
       </c>
-      <c r="C23" t="s">
-        <v>14</v>
-      </c>
-      <c r="D23">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C23" s="3">
+        <v>43739</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B24">
         <v>71.400000000000006</v>
       </c>
-      <c r="C24" t="s">
-        <v>15</v>
-      </c>
-      <c r="D24">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C24" s="3">
+        <v>43770</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B25">
         <v>95.3</v>
       </c>
-      <c r="C25" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C25" s="3">
+        <v>43800</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B26">
         <v>26.6</v>
       </c>
-      <c r="C26" t="s">
-        <v>5</v>
-      </c>
-      <c r="D26">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C26" s="3">
+        <v>43831</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B27">
         <v>58.4</v>
       </c>
-      <c r="C27" t="s">
-        <v>6</v>
-      </c>
-      <c r="D27">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C27" s="3">
+        <v>43862</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B28">
         <v>43.4</v>
       </c>
-      <c r="C28" t="s">
-        <v>7</v>
-      </c>
-      <c r="D28">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C28" s="3">
+        <v>43891</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B29">
         <v>12.7</v>
       </c>
-      <c r="C29" t="s">
-        <v>8</v>
-      </c>
-      <c r="D29">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C29" s="3">
+        <v>43922</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B30">
         <v>14.2</v>
       </c>
-      <c r="C30" t="s">
-        <v>9</v>
-      </c>
-      <c r="D30">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C30" s="3">
+        <v>43952</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B31">
         <v>30.2</v>
       </c>
-      <c r="C31" t="s">
-        <v>10</v>
-      </c>
-      <c r="D31">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C31" s="3">
+        <v>43983</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B32">
         <v>149.30000000000001</v>
       </c>
-      <c r="C32" t="s">
-        <v>11</v>
-      </c>
-      <c r="D32">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C32" s="3">
+        <v>44013</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B33">
         <v>290.2</v>
       </c>
-      <c r="C33" t="s">
-        <v>12</v>
-      </c>
-      <c r="D33">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C33" s="3">
+        <v>44044</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B34">
         <v>49.4</v>
       </c>
-      <c r="C34" t="s">
-        <v>13</v>
-      </c>
-      <c r="D34">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C34" s="3">
+        <v>44075</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B35">
         <v>183.6</v>
       </c>
-      <c r="C35" t="s">
-        <v>14</v>
-      </c>
-      <c r="D35">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C35" s="3">
+        <v>44105</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B36">
         <v>324.10000000000002</v>
       </c>
-      <c r="C36" t="s">
-        <v>15</v>
-      </c>
-      <c r="D36">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C36" s="3">
+        <v>44136</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B37">
         <v>29.5</v>
       </c>
-      <c r="C37" t="s">
-        <v>16</v>
-      </c>
-      <c r="D37">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C37" s="3">
+        <v>44166</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B38">
         <v>1.4</v>
       </c>
-      <c r="C38" t="s">
-        <v>5</v>
-      </c>
-      <c r="D38">
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C38" s="3">
+        <v>44197</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B39">
         <v>45.8</v>
       </c>
-      <c r="C39" t="s">
-        <v>6</v>
-      </c>
-      <c r="D39">
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C39" s="3">
+        <v>44228</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B40">
         <v>75.599999999999994</v>
       </c>
-      <c r="C40" t="s">
-        <v>7</v>
-      </c>
-      <c r="D40">
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C40" s="3">
+        <v>44256</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B41">
         <v>131.6</v>
       </c>
-      <c r="C41" t="s">
-        <v>8</v>
-      </c>
-      <c r="D41">
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C41" s="3">
+        <v>44287</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B42">
         <v>51.5</v>
       </c>
-      <c r="C42" t="s">
-        <v>9</v>
-      </c>
-      <c r="D42">
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C42" s="3">
+        <v>44317</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B43">
         <v>223.1</v>
       </c>
-      <c r="C43" t="s">
-        <v>10</v>
-      </c>
-      <c r="D43">
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C43" s="3">
+        <v>44348</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B44">
         <v>101.9</v>
       </c>
-      <c r="C44" t="s">
-        <v>11</v>
-      </c>
-      <c r="D44">
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C44" s="3">
+        <v>44378</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B45">
         <v>339.7</v>
       </c>
-      <c r="C45" t="s">
-        <v>12</v>
-      </c>
-      <c r="D45">
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C45" s="3">
+        <v>44409</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B46">
         <v>63.2</v>
       </c>
-      <c r="C46" t="s">
-        <v>13</v>
-      </c>
-      <c r="D46">
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C46" s="3">
+        <v>44440</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B47">
         <v>184.4</v>
       </c>
-      <c r="C47" t="s">
-        <v>14</v>
-      </c>
-      <c r="D47">
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C47" s="3">
+        <v>44470</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B48">
         <v>35.200000000000003</v>
       </c>
-      <c r="C48" t="s">
-        <v>15</v>
-      </c>
-      <c r="D48">
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C48" s="3">
+        <v>44501</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B49">
         <v>41.1</v>
       </c>
-      <c r="C49" t="s">
-        <v>16</v>
-      </c>
-      <c r="D49">
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C49" s="3">
+        <v>44531</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B50">
         <v>21.2</v>
       </c>
-      <c r="C50" t="s">
-        <v>5</v>
-      </c>
-      <c r="D50">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C50" s="3">
+        <v>44562</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B51">
         <v>53.7</v>
       </c>
-      <c r="C51" t="s">
-        <v>6</v>
-      </c>
-      <c r="D51">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C51" s="3">
+        <v>44593</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B52">
         <v>218.7</v>
       </c>
-      <c r="C52" t="s">
-        <v>7</v>
-      </c>
-      <c r="D52">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C52" s="3">
+        <v>44621</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>4</v>
-      </c>
-      <c r="B53" s="3">
+        <v>1</v>
+      </c>
+      <c r="B53" s="2">
         <v>194</v>
       </c>
-      <c r="C53" t="s">
-        <v>17</v>
-      </c>
-      <c r="D53">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C53" s="3">
+        <v>44652</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B54">
         <v>78.8</v>
       </c>
-      <c r="C54" t="s">
-        <v>9</v>
-      </c>
-      <c r="D54">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C54" s="3">
+        <v>44682</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B55">
         <v>87.1</v>
       </c>
-      <c r="C55" t="s">
-        <v>18</v>
-      </c>
-      <c r="D55">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C55" s="3">
+        <v>44713</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B56">
         <v>203.2</v>
       </c>
-      <c r="C56" t="s">
-        <v>11</v>
-      </c>
-      <c r="D56">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C56" s="3">
+        <v>44743</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B57">
         <v>153.1</v>
       </c>
-      <c r="C57" t="s">
-        <v>12</v>
-      </c>
-      <c r="D57">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C57" s="3">
+        <v>44774</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B58">
         <v>194.1</v>
       </c>
-      <c r="C58" t="s">
-        <v>13</v>
-      </c>
-      <c r="D58">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C58" s="3">
+        <v>44805</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B59">
         <v>215.9</v>
       </c>
-      <c r="C59" t="s">
-        <v>14</v>
-      </c>
-      <c r="D59">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C59" s="3">
+        <v>44835</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B60">
         <v>215.7</v>
       </c>
-      <c r="C60" t="s">
-        <v>15</v>
-      </c>
-      <c r="D60">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C60" s="3">
+        <v>44866</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>4</v>
-      </c>
-      <c r="B61" s="3">
+        <v>1</v>
+      </c>
+      <c r="B61" s="2">
         <v>30</v>
       </c>
-      <c r="C61" t="s">
-        <v>19</v>
-      </c>
-      <c r="D61">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C61" s="3">
+        <v>44896</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B62">
         <v>39.4</v>
       </c>
-      <c r="C62" t="s">
-        <v>5</v>
-      </c>
-      <c r="D62">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C62" s="3">
+        <v>44927</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B63">
         <v>9.1999999999999993</v>
       </c>
-      <c r="C63" t="s">
-        <v>6</v>
-      </c>
-      <c r="D63">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C63" s="3">
+        <v>44958</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B64">
         <v>10.7</v>
       </c>
-      <c r="C64" t="s">
-        <v>7</v>
-      </c>
-      <c r="D64">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C64" s="3">
+        <v>44986</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B65">
         <v>167</v>
       </c>
-      <c r="C65" t="s">
-        <v>8</v>
-      </c>
-      <c r="D65">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C65" s="3">
+        <v>45017</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B66">
         <v>122.9</v>
       </c>
-      <c r="C66" t="s">
-        <v>9</v>
-      </c>
-      <c r="D66">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C66" s="3">
+        <v>45047</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B67">
         <v>63.8</v>
       </c>
-      <c r="C67" t="s">
-        <v>10</v>
-      </c>
-      <c r="D67">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C67" s="3">
+        <v>45078</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B68">
         <v>180.9</v>
       </c>
-      <c r="C68" t="s">
-        <v>11</v>
-      </c>
-      <c r="D68">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C68" s="3">
+        <v>45108</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B69">
         <v>420.9</v>
       </c>
-      <c r="C69" t="s">
-        <v>12</v>
-      </c>
-      <c r="D69">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C69" s="3">
+        <v>45139</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B70">
         <v>189.5</v>
       </c>
-      <c r="C70" t="s">
-        <v>13</v>
-      </c>
-      <c r="D70">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C70" s="3">
+        <v>45170</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B71">
         <v>75.2</v>
       </c>
-      <c r="C71" t="s">
-        <v>14</v>
-      </c>
-      <c r="D71">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C71" s="3">
+        <v>45200</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B72">
         <v>405.7</v>
       </c>
-      <c r="C72" t="s">
-        <v>15</v>
-      </c>
-      <c r="D72">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C72" s="3">
+        <v>45231</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B73">
         <v>67.2</v>
       </c>
-      <c r="C73" t="s">
-        <v>19</v>
-      </c>
-      <c r="D73">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C73" s="3">
+        <v>45261</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B74">
         <v>20.399999999999999</v>
       </c>
-      <c r="C74" t="s">
-        <v>5</v>
-      </c>
-      <c r="D74">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C74" s="3">
+        <v>45292</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B75">
         <v>30.3</v>
       </c>
-      <c r="C75" t="s">
-        <v>6</v>
-      </c>
-      <c r="D75">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C75" s="3">
+        <v>45323</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B76">
         <v>42.5</v>
       </c>
-      <c r="C76" t="s">
-        <v>20</v>
-      </c>
-      <c r="D76">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C76" s="3">
+        <v>45352</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B77">
         <v>233.6</v>
       </c>
-      <c r="C77" t="s">
-        <v>8</v>
-      </c>
-      <c r="D77">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C77" s="3">
+        <v>45383</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B78">
         <v>273</v>
       </c>
-      <c r="C78" t="s">
-        <v>9</v>
-      </c>
-      <c r="D78">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C78" s="3">
+        <v>45413</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B79">
         <v>177.2</v>
       </c>
-      <c r="C79" t="s">
-        <v>10</v>
-      </c>
-      <c r="D79">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>4</v>
-      </c>
-      <c r="B80">
-        <v>317.89999999999998</v>
-      </c>
-      <c r="C80" t="s">
-        <v>11</v>
-      </c>
-      <c r="D80">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>4</v>
-      </c>
-      <c r="B81">
-        <v>51.9</v>
-      </c>
-      <c r="C81" t="s">
-        <v>12</v>
-      </c>
-      <c r="D81">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>4</v>
-      </c>
-      <c r="B82">
-        <v>162.9</v>
-      </c>
-      <c r="C82" t="s">
-        <v>13</v>
-      </c>
-      <c r="D82">
-        <v>2024</v>
+      <c r="C79" s="3">
+        <v>45444</v>
       </c>
     </row>
   </sheetData>

</xml_diff>